<commit_message>
test: add housing answer test
</commit_message>
<xml_diff>
--- a/tests/answer/case/estimation-housing.test-cases.xlsx
+++ b/tests/answer/case/estimation-housing.test-cases.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/cfp-calc/tests/answer/case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B81EA3-C6BB-FD4F-9629-979C682BA866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A761E6D-360C-2B41-A39E-AB55CA1B711C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44400" yWindow="-2000" windowWidth="38400" windowHeight="23500" activeTab="6" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="52180" yWindow="5300" windowWidth="38400" windowHeight="23500" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="answers" sheetId="48" r:id="rId1"/>
+    <sheet name="answers" sheetId="54" r:id="rId1"/>
     <sheet name="housingA1" sheetId="47" r:id="rId2"/>
     <sheet name="housingA2" sheetId="49" r:id="rId3"/>
     <sheet name="housingA3" sheetId="50" r:id="rId4"/>
@@ -1555,7 +1555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
@@ -1625,7 +1625,7 @@
         <xdr:cNvPr id="2" name="テキスト ボックス 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A862B722-94A0-9442-9AF1-ABF05176F7C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2876717-6ED1-F847-8B62-F0F6BEE7A58F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,7 +1633,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9436100" y="2679700"/>
+          <a:off x="9436100" y="12585700"/>
           <a:ext cx="7645939" cy="6036140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2737,14 +2737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE41DB3E-D541-524E-96DC-8C6FE4B43E8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711EC54F-669E-3C43-9381-2BFF7A31D0D0}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:F340"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -28472,7 +28472,7 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>